<commit_message>
Nick Edits Nanoracks Safety Data Pacakage
</commit_message>
<xml_diff>
--- a/Ground Segment/COMMS -- GS 2019/Link Budget/UHF-LinkBudget-Western.xlsx
+++ b/Ground Segment/COMMS -- GS 2019/Link Budget/UHF-LinkBudget-Western.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca.sharepoint.com/sites/SabarinathanLaboratory/Shared Documents/CubeSat/Comms/Link Budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Mitchell\Documents\Cubesat\Github documents\CubeSat\Ground Segment\COMMS -- GS 2019\Link Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{1409C5AC-B512-4B9C-8E10-7B6B7599D5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{543B5F14-E07A-44B5-B861-ECFDA8C72B67}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277198EA-B979-47E3-A598-373F4D8EA5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-96" windowWidth="22056" windowHeight="13152" tabRatio="850" activeTab="3" xr2:uid="{293003C9-1163-4E50-8A98-C049B95988DD}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" tabRatio="850" activeTab="3" xr2:uid="{293003C9-1163-4E50-8A98-C049B95988DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -222,6 +223,107 @@
         </r>
       </text>
     </comment>
+    <comment ref="V25" authorId="0" shapeId="0" xr:uid="{44A6C021-44D4-4E15-9258-8BB524F5BFFF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nicholas Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Connector Losses assumed to be 0.1 dB each (fairly large) 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V26" authorId="0" shapeId="0" xr:uid="{61355283-EED2-4008-97B0-AD1A7E626F5E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nicholas Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Needs to be taken into account by capstone students
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V27" authorId="0" shapeId="0" xr:uid="{E8097769-D31F-40F0-8225-B87F306D536F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nicholas Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Capstone students, 
+Likely for PA, LNA, Surge protector and isolator</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V28" authorId="0" shapeId="0" xr:uid="{BF2DDE5C-4696-4D16-BD01-F31049D27AFF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nicholas Mitchell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Antenna VSWR is 1.5 Maximum
+equal to mismatch loss of 0.177dB 
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Y50" authorId="0" shapeId="0" xr:uid="{9814FF33-AC8F-4CD8-823F-8F90CE8BA65C}">
       <text>
         <r>
@@ -303,8 +405,15 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Comment:
-    Connectors  X  0.05 dB/Con.</t>
+          <t xml:space="preserve">Comment:
+ Antenna connector: SSMCX female?
+(Unsure on this!!)
+MMCX female?
+Transceiver connector: 
+MMCX female
+Need cable from SSMCX to MMCX 
+Assumed to have 0.1 dB of loss per connector for now. 
+</t>
         </r>
       </text>
     </comment>
@@ -328,9 +437,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+For Cable: 
 Maximum VSWR = 1.3
 equivalent of missmatch of : 0.075 dB
 Equivalent of return loss of 17.69dB 
+For Antenna: 
+Maximum VSWR of 1.15 
+mismatch loss of 0.021 dB
 https://www.allaboutcircuits.com/tools/vswr-return-loss-calculator/
 for more info
 </t>
@@ -4630,6 +4743,33 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4657,32 +4797,11 @@
     <xf numFmtId="49" fontId="0" fillId="23" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4695,12 +4814,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -10844,7 +10957,7 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -10994,7 +11107,7 @@
       </c>
       <c r="E9" s="80">
         <f>Transmitters!V64</f>
-        <v>0.39400000000000002</v>
+        <v>0.41500000000000004</v>
       </c>
       <c r="F9" s="98" t="s">
         <v>38</v>
@@ -11032,7 +11145,7 @@
       </c>
       <c r="E11" s="79">
         <f>E7-E9+E10</f>
-        <v>1.1059999999999999</v>
+        <v>1.085</v>
       </c>
       <c r="F11" s="98" t="s">
         <v>44</v>
@@ -11180,7 +11293,7 @@
       </c>
       <c r="E19" s="79">
         <f>E11-SUM(E13:E18)</f>
-        <v>-152.28482821685787</v>
+        <v>-152.30582821685786</v>
       </c>
       <c r="F19" s="98" t="s">
         <v>44</v>
@@ -11272,7 +11385,7 @@
       </c>
       <c r="E24" s="79">
         <f>E8+'Downlink Budget'!E10+'Downlink Budget'!E21-E9-E15-SUM(E13:E14,E16:E18)-Receivers!V77</f>
-        <v>-111.03127821685786</v>
+        <v>-111.05227821685787</v>
       </c>
       <c r="F24" s="98" t="s">
         <v>216</v>
@@ -11314,7 +11427,7 @@
       </c>
       <c r="E26" s="79">
         <f>E24-E25</f>
-        <v>16.737055225856949</v>
+        <v>16.716055225856934</v>
       </c>
       <c r="F26" s="98" t="s">
         <v>38</v>
@@ -11352,7 +11465,7 @@
       </c>
       <c r="E28" s="192">
         <f>E26-E27</f>
-        <v>3.5870552258569486</v>
+        <v>3.5660552258569336</v>
       </c>
       <c r="F28" s="98" t="s">
         <v>38</v>
@@ -11483,7 +11596,7 @@
       </c>
       <c r="E35" s="117">
         <f>E19-E30-Inputs!V10+E34</f>
-        <v>61.694489221460387</v>
+        <v>61.6734892214604</v>
       </c>
       <c r="F35" s="97" t="s">
         <v>191</v>
@@ -11538,7 +11651,7 @@
       </c>
       <c r="E38" s="117">
         <f>E35-E37</f>
-        <v>21.871776891064705</v>
+        <v>21.850776891064719</v>
       </c>
       <c r="F38" s="97" t="s">
         <v>38</v>
@@ -11593,7 +11706,7 @@
       </c>
       <c r="E41" s="204">
         <f>E38-E40</f>
-        <v>8.7217768910647049</v>
+        <v>8.7007768910647183</v>
       </c>
       <c r="F41" s="112" t="s">
         <v>38</v>
@@ -11629,7 +11742,7 @@
       </c>
       <c r="E43" s="121">
         <f>IF((E28)&lt;0,"Link not completed!",((E22)*LOG((1+E28),2)))</f>
-        <v>54939.206921328157</v>
+        <v>54773.707722026942</v>
       </c>
       <c r="F43" s="122" t="s">
         <v>117</v>
@@ -16080,11 +16193,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="325" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="323"/>
-      <c r="C1" s="323"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
       <c r="D1" s="229"/>
       <c r="F1" s="251"/>
     </row>
@@ -16172,10 +16285,10 @@
       <c r="A10" s="250" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="324" t="s">
+      <c r="B10" s="326" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="324"/>
+      <c r="C10" s="326"/>
       <c r="D10" s="229"/>
     </row>
     <row r="11" spans="1:6" s="231" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -16207,11 +16320,11 @@
       <c r="D13" s="229"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="325" t="s">
+      <c r="A14" s="327" t="s">
         <v>343</v>
       </c>
-      <c r="B14" s="325"/>
-      <c r="C14" s="325"/>
+      <c r="B14" s="327"/>
+      <c r="C14" s="327"/>
       <c r="D14" s="229"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -16278,10 +16391,10 @@
       <c r="A21" s="253" t="s">
         <v>341</v>
       </c>
-      <c r="B21" s="326" t="s">
+      <c r="B21" s="328" t="s">
         <v>359</v>
       </c>
-      <c r="C21" s="326"/>
+      <c r="C21" s="328"/>
       <c r="D21" s="229"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -16313,11 +16426,11 @@
       <c r="D24" s="229"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="323" t="s">
+      <c r="A25" s="325" t="s">
         <v>362</v>
       </c>
-      <c r="B25" s="323"/>
-      <c r="C25" s="323"/>
+      <c r="B25" s="325"/>
+      <c r="C25" s="325"/>
       <c r="D25" s="229"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -16374,10 +16487,10 @@
       <c r="A31" s="250" t="s">
         <v>371</v>
       </c>
-      <c r="B31" s="327" t="s">
+      <c r="B31" s="323" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="328"/>
+      <c r="C31" s="324"/>
       <c r="D31" s="229"/>
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -16409,22 +16522,22 @@
       <c r="D34" s="229"/>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="315" t="s">
+      <c r="A35" s="306" t="s">
         <v>375</v>
       </c>
-      <c r="B35" s="315"/>
-      <c r="C35" s="315"/>
-      <c r="D35" s="315"/>
+      <c r="B35" s="306"/>
+      <c r="C35" s="306"/>
+      <c r="D35" s="306"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="316" t="s">
+      <c r="A36" s="307" t="s">
         <v>376</v>
       </c>
-      <c r="B36" s="317"/>
-      <c r="C36" s="318" t="s">
+      <c r="B36" s="308"/>
+      <c r="C36" s="309" t="s">
         <v>377</v>
       </c>
-      <c r="D36" s="319"/>
+      <c r="D36" s="310"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="257" t="s">
@@ -16483,12 +16596,12 @@
       <c r="D42" s="260"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="320" t="s">
+      <c r="A43" s="311" t="s">
         <v>341</v>
       </c>
-      <c r="B43" s="321"/>
-      <c r="C43" s="321"/>
-      <c r="D43" s="322"/>
+      <c r="B43" s="312"/>
+      <c r="C43" s="312"/>
+      <c r="D43" s="313"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="257" t="s">
@@ -16580,27 +16693,27 @@
       <c r="A51" s="257" t="s">
         <v>431</v>
       </c>
-      <c r="B51" s="308" t="s">
+      <c r="B51" s="317" t="s">
         <v>432</v>
       </c>
-      <c r="C51" s="309"/>
-      <c r="D51" s="310"/>
+      <c r="C51" s="318"/>
+      <c r="D51" s="319"/>
     </row>
     <row r="52" spans="1:4" s="231" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="257" t="s">
         <v>434</v>
       </c>
-      <c r="B52" s="308" t="s">
+      <c r="B52" s="317" t="s">
         <v>433</v>
       </c>
-      <c r="C52" s="309"/>
-      <c r="D52" s="310"/>
+      <c r="C52" s="318"/>
+      <c r="D52" s="319"/>
     </row>
     <row r="53" spans="1:4" s="231" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="259"/>
-      <c r="B53" s="311"/>
-      <c r="C53" s="312"/>
-      <c r="D53" s="313"/>
+      <c r="B53" s="320"/>
+      <c r="C53" s="321"/>
+      <c r="D53" s="322"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="229"/>
@@ -16609,11 +16722,11 @@
       <c r="D54" s="229"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="314" t="s">
+      <c r="A55" s="305" t="s">
         <v>402</v>
       </c>
-      <c r="B55" s="314"/>
-      <c r="C55" s="314"/>
+      <c r="B55" s="305"/>
+      <c r="C55" s="305"/>
       <c r="D55" s="229"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -16709,11 +16822,11 @@
       <c r="D65" s="229"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="314" t="s">
+      <c r="A66" s="305" t="s">
         <v>418</v>
       </c>
-      <c r="B66" s="314"/>
-      <c r="C66" s="314"/>
+      <c r="B66" s="305"/>
+      <c r="C66" s="305"/>
       <c r="D66" s="229"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -16733,7 +16846,7 @@
       <c r="B68" s="264" t="s">
         <v>421</v>
       </c>
-      <c r="C68" s="305" t="s">
+      <c r="C68" s="314" t="s">
         <v>420</v>
       </c>
       <c r="D68" s="229"/>
@@ -16745,7 +16858,7 @@
       <c r="B69" s="264" t="s">
         <v>422</v>
       </c>
-      <c r="C69" s="306"/>
+      <c r="C69" s="315"/>
       <c r="D69" s="229"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -16755,7 +16868,7 @@
       <c r="B70" s="264">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C70" s="306"/>
+      <c r="C70" s="315"/>
       <c r="D70" s="229"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -16765,7 +16878,7 @@
       <c r="B71" s="264" t="s">
         <v>423</v>
       </c>
-      <c r="C71" s="306"/>
+      <c r="C71" s="315"/>
       <c r="D71" s="229"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -16775,7 +16888,7 @@
       <c r="B72" s="264" t="s">
         <v>423</v>
       </c>
-      <c r="C72" s="306"/>
+      <c r="C72" s="315"/>
       <c r="D72" s="229"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -16785,7 +16898,7 @@
       <c r="B73" s="265" t="s">
         <v>412</v>
       </c>
-      <c r="C73" s="306"/>
+      <c r="C73" s="315"/>
       <c r="D73" s="229"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -16795,7 +16908,7 @@
       <c r="B74" s="264" t="s">
         <v>425</v>
       </c>
-      <c r="C74" s="307"/>
+      <c r="C74" s="316"/>
       <c r="D74" s="229"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -16815,11 +16928,11 @@
       <c r="D76" s="229"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="314" t="s">
+      <c r="A77" s="305" t="s">
         <v>458</v>
       </c>
-      <c r="B77" s="314"/>
-      <c r="C77" s="314"/>
+      <c r="B77" s="305"/>
+      <c r="C77" s="305"/>
       <c r="D77" s="229"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -16903,11 +17016,11 @@
       <c r="D84" s="229"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="314" t="s">
+      <c r="A85" s="305" t="s">
         <v>462</v>
       </c>
-      <c r="B85" s="314"/>
-      <c r="C85" s="314"/>
+      <c r="B85" s="305"/>
+      <c r="C85" s="305"/>
       <c r="D85" s="229"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -17021,8 +17134,8 @@
   </sheetPr>
   <dimension ref="A1:AQ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32:W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.7" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -18117,7 +18230,9 @@
       <c r="S24" s="330"/>
       <c r="T24" s="330"/>
       <c r="U24" s="331"/>
-      <c r="V24" s="333"/>
+      <c r="V24" s="333">
+        <v>2</v>
+      </c>
       <c r="W24" s="333"/>
       <c r="X24" s="333"/>
       <c r="Y24" s="32" t="s">
@@ -18166,7 +18281,9 @@
       <c r="S25" s="330"/>
       <c r="T25" s="330"/>
       <c r="U25" s="334"/>
-      <c r="V25" s="335"/>
+      <c r="V25" s="335">
+        <v>0.1</v>
+      </c>
       <c r="W25" s="335"/>
       <c r="X25" s="335"/>
       <c r="Y25" s="32" t="s">
@@ -18313,7 +18430,9 @@
       <c r="S28" s="330"/>
       <c r="T28" s="330"/>
       <c r="U28" s="331"/>
-      <c r="V28" s="333"/>
+      <c r="V28" s="333">
+        <v>0.17699999999999999</v>
+      </c>
       <c r="W28" s="333"/>
       <c r="X28" s="333"/>
       <c r="Y28" s="32" t="s">
@@ -18455,8 +18574,8 @@
       </c>
       <c r="U31" s="331"/>
       <c r="V31" s="335">
-        <f>T21+SUM(V25:X28)</f>
-        <v>0.40094999999999997</v>
+        <f>T21+SUM(V26:X28)+V24*V25</f>
+        <v>0.77794999999999992</v>
       </c>
       <c r="W31" s="335"/>
       <c r="X31" s="32" t="s">
@@ -18508,7 +18627,7 @@
       <c r="U32" s="331"/>
       <c r="V32" s="335">
         <f>T16-V31</f>
-        <v>-0.40094999999999997</v>
+        <v>-0.77794999999999992</v>
       </c>
       <c r="W32" s="345"/>
       <c r="X32" s="32" t="s">
@@ -19701,7 +19820,7 @@
       <c r="T57" s="336"/>
       <c r="U57" s="336"/>
       <c r="V57" s="339">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W57" s="340"/>
       <c r="X57" s="341"/>
@@ -19752,7 +19871,7 @@
       <c r="T58" s="336"/>
       <c r="U58" s="336"/>
       <c r="V58" s="342">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="W58" s="343"/>
       <c r="X58" s="344"/>
@@ -19905,7 +20024,8 @@
       <c r="T61" s="336"/>
       <c r="U61" s="336"/>
       <c r="V61" s="339">
-        <v>7.4999999999999997E-2</v>
+        <f>0.075+0.021</f>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="W61" s="340"/>
       <c r="X61" s="341"/>
@@ -20048,8 +20168,8 @@
       </c>
       <c r="U64" s="336"/>
       <c r="V64" s="337">
-        <f>T54+SUM(V58:X61)</f>
-        <v>0.39400000000000002</v>
+        <f>T54+SUM(V59:X61)+V57*V58</f>
+        <v>0.41500000000000004</v>
       </c>
       <c r="W64" s="338"/>
       <c r="X64" s="41" t="s">
@@ -20101,7 +20221,7 @@
       <c r="U65" s="336"/>
       <c r="V65" s="337">
         <f>T49-V64</f>
-        <v>-0.39400000000000002</v>
+        <v>-0.41500000000000004</v>
       </c>
       <c r="W65" s="338"/>
       <c r="X65" s="41" t="s">
@@ -20335,7 +20455,7 @@
   </sheetPr>
   <dimension ref="A1:AX58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
@@ -23105,8 +23225,8 @@
   </sheetPr>
   <dimension ref="A1:AQ91"/>
   <sheetViews>
-    <sheetView topLeftCell="L64" zoomScale="104" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="V74" sqref="V74:X74"/>
+    <sheetView topLeftCell="L70" zoomScale="104" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="Z67" sqref="Z67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.7" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -28918,7 +29038,7 @@
   </sheetPr>
   <dimension ref="A1:AQ108"/>
   <sheetViews>
-    <sheetView topLeftCell="E85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="U100" sqref="U100"/>
     </sheetView>
   </sheetViews>
@@ -34237,7 +34357,7 @@
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -34396,7 +34516,7 @@
       </c>
       <c r="E9" s="79">
         <f>Transmitters!V31</f>
-        <v>0.40094999999999997</v>
+        <v>0.77794999999999992</v>
       </c>
       <c r="F9" s="98" t="s">
         <v>38</v>
@@ -34436,7 +34556,7 @@
       </c>
       <c r="E11" s="79">
         <f>E7-E9+E10</f>
-        <v>12.899050000000001</v>
+        <v>12.52205</v>
       </c>
       <c r="F11" s="98" t="s">
         <v>44</v>
@@ -34590,7 +34710,7 @@
       </c>
       <c r="E19" s="79">
         <f>E11-SUM(E13:E18)</f>
-        <v>-140.49177821685788</v>
+        <v>-140.86877821685786</v>
       </c>
       <c r="F19" s="98" t="s">
         <v>44</v>
@@ -34718,7 +34838,7 @@
       </c>
       <c r="E26" s="79">
         <f>E19-E21+E22-E23</f>
-        <v>-139.6917782168579</v>
+        <v>-140.06877821685788</v>
       </c>
       <c r="F26" s="98" t="s">
         <v>44</v>
@@ -34775,7 +34895,7 @@
       </c>
       <c r="E29" s="79">
         <f>E26-E28</f>
-        <v>19.709276873040409</v>
+        <v>19.332276873040428</v>
       </c>
       <c r="F29" s="98" t="s">
         <v>38</v>
@@ -34815,7 +34935,7 @@
       </c>
       <c r="E31" s="204">
         <f>IF((E29-E30)&lt;0,"Link not completed!",E29-E30)</f>
-        <v>5.8092768730404085</v>
+        <v>5.4322768730404274</v>
       </c>
       <c r="F31" s="98" t="s">
         <v>38</v>
@@ -34946,7 +35066,7 @@
       </c>
       <c r="E38" s="117">
         <f>E19-E33-Inputs!V10+E37</f>
-        <v>63.888676959760801</v>
+        <v>63.51167695976082</v>
       </c>
       <c r="F38" s="97" t="s">
         <v>191</v>
@@ -35001,7 +35121,7 @@
       </c>
       <c r="E41" s="117">
         <f>E38-E40</f>
-        <v>24.065964629365119</v>
+        <v>23.688964629365138</v>
       </c>
       <c r="F41" s="97" t="s">
         <v>38</v>
@@ -35056,7 +35176,7 @@
       </c>
       <c r="E44" s="204">
         <f>IF((E41-E43)&lt;0,"Link not completed!",E41-E43)</f>
-        <v>10.165964629365119</v>
+        <v>9.7889646293651378</v>
       </c>
       <c r="F44" s="112" t="s">
         <v>38</v>
@@ -35092,7 +35212,7 @@
       </c>
       <c r="E46" s="121">
         <f>IF(E44&lt;0,"Link not completed!",((E27)*LOG((1+E44),2)))</f>
-        <v>87025.899651835251</v>
+        <v>85787.112927606984</v>
       </c>
       <c r="F46" s="122" t="s">
         <v>117</v>

</xml_diff>